<commit_message>
fix: change up to mid cap
</commit_message>
<xml_diff>
--- a/data/up_to_mid.xlsx
+++ b/data/up_to_mid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>up-9</t>
   </si>
@@ -34,6 +34,9 @@
     <t>mid-2</t>
   </si>
   <si>
+    <t>48.259</t>
+  </si>
+  <si>
     <t>2410.5655</t>
   </si>
   <si>
@@ -49,7 +52,7 @@
     <t>mid-4</t>
   </si>
   <si>
-    <t>800</t>
+    <t>22.171</t>
   </si>
   <si>
     <t>3147.0030</t>
@@ -58,6 +61,9 @@
     <t>mid-5</t>
   </si>
   <si>
+    <t>224.341</t>
+  </si>
+  <si>
     <t>1946.8041</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t>mid-6</t>
   </si>
   <si>
+    <t>139.261</t>
+  </si>
+  <si>
     <t>368.9537</t>
   </si>
   <si>
@@ -76,24 +85,36 @@
     <t>mid-7</t>
   </si>
   <si>
+    <t>123.703</t>
+  </si>
+  <si>
     <t>1476.4894</t>
   </si>
   <si>
     <t>mid-8</t>
   </si>
   <si>
+    <t>200.571</t>
+  </si>
+  <si>
     <t>1237.0542</t>
   </si>
   <si>
     <t>mid-9</t>
   </si>
   <si>
+    <t>112.849</t>
+  </si>
+  <si>
     <t>1492.4167</t>
   </si>
   <si>
     <t>mid-10</t>
   </si>
   <si>
+    <t>151.427</t>
+  </si>
+  <si>
     <t>1121.3613</t>
   </si>
   <si>
@@ -103,18 +124,27 @@
     <t>mid-11</t>
   </si>
   <si>
+    <t>5.69</t>
+  </si>
+  <si>
     <t>1873.5261</t>
   </si>
   <si>
     <t>mid-12</t>
   </si>
   <si>
+    <t>0.617</t>
+  </si>
+  <si>
     <t>2129.8923</t>
   </si>
   <si>
     <t>mid-13</t>
   </si>
   <si>
+    <t>319.289</t>
+  </si>
+  <si>
     <t>1490.0340</t>
   </si>
   <si>
@@ -124,12 +154,18 @@
     <t>mid-14</t>
   </si>
   <si>
+    <t>253.039</t>
+  </si>
+  <si>
     <t>1193.5749</t>
   </si>
   <si>
     <t>mid-15</t>
   </si>
   <si>
+    <t>250.311</t>
+  </si>
+  <si>
     <t>1341.8415</t>
   </si>
   <si>
@@ -139,18 +175,27 @@
     <t>mid-16</t>
   </si>
   <si>
+    <t>410.517</t>
+  </si>
+  <si>
     <t>1219.9936</t>
   </si>
   <si>
     <t>mid-17</t>
   </si>
   <si>
+    <t>175.847</t>
+  </si>
+  <si>
     <t>1411.6795</t>
   </si>
   <si>
     <t>mid-18</t>
   </si>
   <si>
+    <t>125.506</t>
+  </si>
+  <si>
     <t>1799.9862</t>
   </si>
   <si>
@@ -160,10 +205,16 @@
     <t>mid-19</t>
   </si>
   <si>
+    <t>149.405</t>
+  </si>
+  <si>
     <t>1636.5584</t>
   </si>
   <si>
     <t>mid-20</t>
+  </si>
+  <si>
+    <t>147.022</t>
   </si>
   <si>
     <t>836.9388</t>
@@ -498,10 +549,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -509,27 +560,27 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -537,223 +588,223 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add cars model
</commit_message>
<xml_diff>
--- a/data/up_to_mid.xlsx
+++ b/data/up_to_mid.xlsx
@@ -14,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>cap</t>
+  </si>
+  <si>
+    <t>dis</t>
+  </si>
   <si>
     <t>up-9</t>
   </si>
@@ -557,27 +569,27 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -585,21 +597,21 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -627,49 +639,49 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
@@ -683,35 +695,35 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
@@ -725,21 +737,21 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
         <v>52</v>
@@ -753,35 +765,35 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>62</v>
@@ -795,16 +807,30 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>